<commit_message>
Funcionalidad de Seguimiento SANNA
</commit_message>
<xml_diff>
--- a/templates/Seguimiento_Base.xlsx
+++ b/templates/Seguimiento_Base.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koyuk\Desktop\Pega\SANNA_HECTOR\Proyecto Pentaho\Generar Archivos Sanna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\recaudacion_SANNA\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E923C-29F3-4EBD-BC90-C9C16DC08C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25260" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{62B89059-8C21-49E4-990E-B59498C73D38}"/>
+    <workbookView xWindow="25260" yWindow="-16320" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>A01</t>
   </si>
@@ -97,12 +96,75 @@
   </si>
   <si>
     <t>Castigo por cotizaciones SANNA DNP</t>
+  </si>
+  <si>
+    <t>origen</t>
+  </si>
+  <si>
+    <t>periodo</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>trabajadores_unicos</t>
+  </si>
+  <si>
+    <t>empleadores_unicos</t>
+  </si>
+  <si>
+    <t>planillas_unicas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="42" formatCode="_ &quot;$&quot;* #,##0_ ;_ &quot;$&quot;* \-#,##0_ ;_ &quot;$&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
@@ -531,31 +593,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C619A9-4CFD-48AE-9CE5-95033C63B727}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2:U2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="12" max="13" width="13.109375" customWidth="1"/>
-    <col min="15" max="15" width="12.21875" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="12.21875" customWidth="1"/>
-    <col min="18" max="18" width="13.33203125" customWidth="1"/>
-    <col min="19" max="19" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="12" max="13" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="125.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,30 +682,72 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -666,7 +770,7 @@
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -689,7 +793,7 @@
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
@@ -712,7 +816,7 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14"/>
@@ -735,17 +839,17 @@
       <c r="T6" s="15"/>
       <c r="U6" s="15"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S9" s="17"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S11" s="16"/>
       <c r="T11" s="16"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T12" s="16"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T14" s="16"/>
     </row>
   </sheetData>

</xml_diff>